<commit_message>
FIX parameters to production
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,25 +442,25 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Terapeuta</v>
+        <v>Acompañante de menor o Maestro Sombra</v>
       </c>
       <c r="B2" t="str">
         <v>La empresa es confidencial o no se encuentra disponible</v>
       </c>
       <c r="C2" t="str">
-        <v>León,, Gto.</v>
+        <v>Hermosillo,, Son.</v>
       </c>
       <c r="D2" t="str">
-        <v>$14,000 - $16,000 Mensual</v>
+        <v>$12,000 Mensual</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <v>Sector salud</v>
+        <v>Educación</v>
       </c>
       <c r="G2" t="str">
-        <v>Terapeuta</v>
+        <v>Educación especial</v>
       </c>
       <c r="H2" t="str">
         <v>Universitario titulado</v>
@@ -475,6 +475,63 @@
         <v>Presencial</v>
       </c>
       <c r="L2" t="str" xml:space="preserve">
+        <v xml:space="preserve">Vacante: Acompañante de niño (TDA o Autismo) – Maestro Sombra
+Ubicación: Zona Poniente, Hermosillo
+Horario: lunes a viernes
+Requisitos:
+Sexo indistinto
+Carrera en Pedagogía, Ciencias de la Educación o afín
+Especialidad o experiencia en Educación Especial
+Experiencia como maestro sombra o acompañante educativo
+Paciencia, empatía y habilidades de comunicación
+Responsabilidad y compromiso
+Preferente cuente con carro para su traslado
+Funciones principales:
+Brindar apoyo personalizado a un niño con TDA o Trastorno del Espectro Autista en su entorno escolar
+Favorecer la integración e inclusión en actividades académicas y sociales
+Implementar estrategias de apoyo de acuerdo con el plan educativo
+Colaborar con docentes y padres para dar seguimiento al progreso
+Ofrecemos:
+Contratación directa
+Estabilidad laboral
+Ambiente de trabajo respetuoso y colaborativo</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>Terapeuta</v>
+      </c>
+      <c r="B3" t="str">
+        <v>La empresa es confidencial o no se encuentra disponible</v>
+      </c>
+      <c r="C3" t="str">
+        <v>León,, Gto.</v>
+      </c>
+      <c r="D3" t="str">
+        <v>$14,000 - $16,000 Mensual</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Sector salud</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Terapeuta</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Presencial</v>
+      </c>
+      <c r="L3" t="str" xml:space="preserve">
         <v xml:space="preserve">Requisitos del puesto
 Estudios universitarios con título en Terapia.
 Experiencia previa como Terapeuta de niños con Trastornos del espectro autista.
@@ -494,58 +551,6 @@
 Vales de despensa.
 Fondo de ahorro.
 Oportunidades de capacitación y desarrollo profesional en un ambiente de trabajo colaborativo y en constante crecimiento.</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>Psicóloga</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Neuro Activa</v>
-      </c>
-      <c r="C3" t="str">
-        <v>CDMX</v>
-      </c>
-      <c r="D3" t="str">
-        <v>$8,364 - $8,500 Mensual</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Educación</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Psicopedagogía</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Universitario titulado</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Permanente</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Tiempo completo</v>
-      </c>
-      <c r="K3" t="str">
-        <v>Híbrido</v>
-      </c>
-      <c r="L3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Acerca de la empresa
-Neuro Activa es una empresa líder en el campo de la educación y la psicopedagogía, comprometida con el desarrollo integral de cada individuo. Trabajar con nosotros significa formar parte de un equipo dedicado a brindar soluciones innovadoras y personalizadas a las necesidades educativas especiales. - Ubicación: Ciudad de México.
-Requisitos del puesto
-Licenciatura en Psicología, Educación Especial, Pedagogía, Psicopedagogía o afines.
-Diplomado o curso en intervención educativa, inclusión escolar o TEA/TDAH. (Deseable)
-Experiencia mínima de 6 meses con niños con necesidades educativas especiales (NEE), Trastorno del Espectro Autista (TEA), TDAH u otras condiciones del neurodesarrollo.
-Conocimientos básicos de adaptaciones curriculares y manejo de conductas.
-Habilidades en regulación emocional, contención y acompañamiento respetuoso.
-Capacidad para implementar estrategias sensoriales, estructuración del entorno y apoyos visuales.
-Buen manejo de la comunicación con familia y equipo docente.
-Responsabilidades del puesto
-Brindar intervención educativa y apoyo a niños con necesidades educativas especiales.
-Implementar estrategias de inclusión escolar y adaptaciones curriculares.
-Colaborar con el equipo docente y familia en el desarrollo del plan de intervención individualizado.
-Únete a nuestro equipo en Neuro Activa y sé parte de un proyecto que transforma vidas a través de la educación inclusiva. ¡Aplica ahora y haz la diferencia!</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
@@ -657,16 +662,16 @@
     </row>
     <row r="6" xml:space="preserve">
       <c r="A6" t="str">
-        <v>Maestra</v>
+        <v>Psicóloga</v>
       </c>
       <c r="B6" t="str">
-        <v>Asociación Centro de T...</v>
+        <v>Neuro Activa</v>
       </c>
       <c r="C6" t="str">
-        <v>SLP.</v>
+        <v>CDMX</v>
       </c>
       <c r="D6" t="str">
-        <v>$5,000 - $6,000 Mensual</v>
+        <v>$8,364 - $8,500 Mensual</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -675,7 +680,7 @@
         <v>Educación</v>
       </c>
       <c r="G6" t="str">
-        <v>Educación especial</v>
+        <v>Psicopedagogía</v>
       </c>
       <c r="H6" t="str">
         <v>Universitario titulado</v>
@@ -684,12 +689,64 @@
         <v>Permanente</v>
       </c>
       <c r="J6" t="str">
-        <v>Medio tiempo</v>
+        <v>Tiempo completo</v>
       </c>
       <c r="K6" t="str">
         <v>Híbrido</v>
       </c>
       <c r="L6" t="str" xml:space="preserve">
+        <v xml:space="preserve">Acerca de la empresa
+Neuro Activa es una empresa líder en el campo de la educación y la psicopedagogía, comprometida con el desarrollo integral de cada individuo. Trabajar con nosotros significa formar parte de un equipo dedicado a brindar soluciones innovadoras y personalizadas a las necesidades educativas especiales. - Ubicación: Ciudad de México.
+Requisitos del puesto
+Licenciatura en Psicología, Educación Especial, Pedagogía, Psicopedagogía o afines.
+Diplomado o curso en intervención educativa, inclusión escolar o TEA/TDAH. (Deseable)
+Experiencia mínima de 6 meses con niños con necesidades educativas especiales (NEE), Trastorno del Espectro Autista (TEA), TDAH u otras condiciones del neurodesarrollo.
+Conocimientos básicos de adaptaciones curriculares y manejo de conductas.
+Habilidades en regulación emocional, contención y acompañamiento respetuoso.
+Capacidad para implementar estrategias sensoriales, estructuración del entorno y apoyos visuales.
+Buen manejo de la comunicación con familia y equipo docente.
+Responsabilidades del puesto
+Brindar intervención educativa y apoyo a niños con necesidades educativas especiales.
+Implementar estrategias de inclusión escolar y adaptaciones curriculares.
+Colaborar con el equipo docente y familia en el desarrollo del plan de intervención individualizado.
+Únete a nuestro equipo en Neuro Activa y sé parte de un proyecto que transforma vidas a través de la educación inclusiva. ¡Aplica ahora y haz la diferencia!</v>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7" t="str">
+        <v>Maestra</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Asociación Centro de T...</v>
+      </c>
+      <c r="C7" t="str">
+        <v>SLP.</v>
+      </c>
+      <c r="D7" t="str">
+        <v>$5,000 - $6,000 Mensual</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Educación</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Educación especial</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Medio tiempo</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Híbrido</v>
+      </c>
+      <c r="L7" t="str" xml:space="preserve">
         <v xml:space="preserve">Acerca de la empresa
 **** Asociación Centro de Terapia Infantil y de Educación Especial es una organización comprometida con el bienestar y desarrollo de niños, niñas y jóvenes con autismo, síndrome de Down y/o discapacidad intelectual. Nuestra misión es brindar un ambiente inclusivo y terapéutico para promover su crecimiento y aprendizaje. - **Ubicación:** San Luis Potosí.
 Requisitos del puesto
@@ -711,7 +768,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>